<commit_message>
Update test log and results
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szenzaro/work/iliad-aligner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnnyfreak/work/unil/new-aligner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEE3162-AE34-F142-BF55-C7D88B1BCB4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637F2DC3-62FC-964D-9C04-5EE0306C3152}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21580" activeTab="1" xr2:uid="{6CA32234-533A-F040-B343-0864799DC979}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{6CA32234-533A-F040-B343-0864799DC979}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
+    <sheet name="Old" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feuil1!$A$1:$H$1</definedName>
-    <definedName name="test" localSheetId="1">Feuil1!$A$1:$H$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,27 +28,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{CACA593C-C29C-2E41-B7BF-C8DA57B70800}" name="test" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/szenzaro/work/iliad-aligner/out/test.log">
-      <textFields count="8">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="449">
   <si>
     <t>editType</t>
   </si>
@@ -1120,6 +1100,282 @@
   </si>
   <si>
     <t xml:space="preserve"> [0.0070276105017222715 0.8606768716527329 0.5077291467486299]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6460053656628086 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9188871234510602 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6873681739259769 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8574268671453509 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7497521526368519 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9322501743166094 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5629823813918866 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9068527115425187 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6632762846628092 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9240069417048102 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7047792560038417 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9025868936055864 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7525143082147384 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9297113096977228 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.47624820403623935 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7259640937230261 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6343997827651935 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.74868675713888 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6904946364445451 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7593995501852593 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.714321577802875 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7642210853976176 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5517043355028848 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.75990761154246 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5325386605097048 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7618125438894303 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7160634737965527 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.769193233983029 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.72428717595435 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7711891126369587 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5649741724254065 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.63835548990645 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7087880323304784 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9518072189561542 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7256243118492236 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.918361243135279 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7865875605698793 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9505866255283796 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.632454221845676 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9470486158352146 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7130144959186367 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.949083164146804 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7454036052621954 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9320768675752146 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7850067271574359 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9500607644179143 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5549582204754243 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7623494950538111 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7020469541898436 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7736952461462133 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [TagDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7391080307422958 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7769439969387832 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13h47m1.81950361s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13h14m32.419081518s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32m29.400421385s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.03412210866900017 0.8689054700780663 0.49204088333844737]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [TextualDistance TagDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7552353220075224 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7798790014373886 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16h12m39.04346299s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15h34m19.244955304s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38m19.798507146s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.01097656583701741 0.03787970522758509 0.8766090534069513 0.4765970760269912]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [VocDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6370588750438223 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7729991399995806 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12h33m58.605620087s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12h4m10.309897748s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29m48.295721869s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.02035422604654383 0.8720346628361442 0.48559330508651743]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [TextualDistance VocDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7110419914437431 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7758024210090432 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15h10m1.966282638s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14h34m15.541667992s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35m46.424613837s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.0015315508626823474 0.02593177292437441 0.863897666866823 0.500617622689461]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [TagDistance VocDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7474546405668967 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7806675108448915 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17h2m25.679607083s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16h12m23.79394223s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50m1.88566408s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.043961759609716246 0.023492108777153013 0.9434342798422645 0.3266090219830218]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [TextualDistance TagDistance VocDistance ScholieDistance EqEquivTermDistance] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.755813993632767 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7896961107777825 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21h32m10.493972486s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20h33m46.643705974s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 58m23.850265831s </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.018152128930971186 0.10553455838275491 0.022886327036365627 0.9372600039747476 0.3281221741624806]</t>
   </si>
 </sst>
 </file>
@@ -1162,11 +1418,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,12 +1441,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test" connectionId="1" xr16:uid="{9F627CAA-BADC-A648-B32C-72724EBE3BA8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1484,10 +1737,874 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CEB70BC-EEE6-BF41-A547-15ABF05BD9E2}">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F3" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E4" t="s">
+        <v>445</v>
+      </c>
+      <c r="F4" t="s">
+        <v>446</v>
+      </c>
+      <c r="G4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>414</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D5" t="s">
+        <v>416</v>
+      </c>
+      <c r="E5" t="s">
+        <v>417</v>
+      </c>
+      <c r="F5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" t="s">
+        <v>266</v>
+      </c>
+      <c r="G6" t="s">
+        <v>267</v>
+      </c>
+      <c r="H6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D7" t="s">
+        <v>362</v>
+      </c>
+      <c r="E7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E8" t="s">
+        <v>438</v>
+      </c>
+      <c r="F8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G8" t="s">
+        <v>440</v>
+      </c>
+      <c r="H8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E9" t="s">
+        <v>338</v>
+      </c>
+      <c r="F9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G9" t="s">
+        <v>340</v>
+      </c>
+      <c r="H9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D10" t="s">
+        <v>409</v>
+      </c>
+      <c r="E10" t="s">
+        <v>410</v>
+      </c>
+      <c r="F10" t="s">
+        <v>411</v>
+      </c>
+      <c r="G10" t="s">
+        <v>412</v>
+      </c>
+      <c r="H10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D11" t="s">
+        <v>392</v>
+      </c>
+      <c r="E11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" t="s">
+        <v>319</v>
+      </c>
+      <c r="G11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D12" t="s">
+        <v>386</v>
+      </c>
+      <c r="E12" t="s">
+        <v>304</v>
+      </c>
+      <c r="F12" t="s">
+        <v>305</v>
+      </c>
+      <c r="G12" t="s">
+        <v>306</v>
+      </c>
+      <c r="H12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>298</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D13" t="s">
+        <v>384</v>
+      </c>
+      <c r="E13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>301</v>
+      </c>
+      <c r="H13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E14" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" t="s">
+        <v>285</v>
+      </c>
+      <c r="G14" t="s">
+        <v>286</v>
+      </c>
+      <c r="H14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D15" t="s">
+        <v>398</v>
+      </c>
+      <c r="E15" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" t="s">
+        <v>335</v>
+      </c>
+      <c r="H15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>428</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D16" t="s">
+        <v>430</v>
+      </c>
+      <c r="E16" t="s">
+        <v>431</v>
+      </c>
+      <c r="F16" t="s">
+        <v>432</v>
+      </c>
+      <c r="G16" t="s">
+        <v>433</v>
+      </c>
+      <c r="H16" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="D17" t="s">
+        <v>390</v>
+      </c>
+      <c r="E17" t="s">
+        <v>313</v>
+      </c>
+      <c r="F17" t="s">
+        <v>314</v>
+      </c>
+      <c r="G17" t="s">
+        <v>315</v>
+      </c>
+      <c r="H17" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D18" t="s">
+        <v>368</v>
+      </c>
+      <c r="E18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F18" t="s">
+        <v>261</v>
+      </c>
+      <c r="G18" t="s">
+        <v>262</v>
+      </c>
+      <c r="H18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D19" t="s">
+        <v>406</v>
+      </c>
+      <c r="E19" t="s">
+        <v>353</v>
+      </c>
+      <c r="F19" t="s">
+        <v>354</v>
+      </c>
+      <c r="G19" t="s">
+        <v>355</v>
+      </c>
+      <c r="H19" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D20" t="s">
+        <v>376</v>
+      </c>
+      <c r="E20" t="s">
+        <v>279</v>
+      </c>
+      <c r="F20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G20" t="s">
+        <v>281</v>
+      </c>
+      <c r="H20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D21" t="s">
+        <v>360</v>
+      </c>
+      <c r="E21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F21" t="s">
+        <v>241</v>
+      </c>
+      <c r="G21" t="s">
+        <v>242</v>
+      </c>
+      <c r="H21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D22" t="s">
+        <v>366</v>
+      </c>
+      <c r="E22" t="s">
+        <v>255</v>
+      </c>
+      <c r="F22" t="s">
+        <v>256</v>
+      </c>
+      <c r="G22" t="s">
+        <v>257</v>
+      </c>
+      <c r="H22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" t="s">
+        <v>358</v>
+      </c>
+      <c r="E23" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" t="s">
+        <v>236</v>
+      </c>
+      <c r="G23" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D24" t="s">
+        <v>423</v>
+      </c>
+      <c r="E24" t="s">
+        <v>424</v>
+      </c>
+      <c r="F24" t="s">
+        <v>425</v>
+      </c>
+      <c r="G24" t="s">
+        <v>426</v>
+      </c>
+      <c r="H24" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D25" t="s">
+        <v>374</v>
+      </c>
+      <c r="E25" t="s">
+        <v>274</v>
+      </c>
+      <c r="F25" t="s">
+        <v>275</v>
+      </c>
+      <c r="G25" t="s">
+        <v>276</v>
+      </c>
+      <c r="H25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>327</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="D26" t="s">
+        <v>396</v>
+      </c>
+      <c r="E26" t="s">
+        <v>328</v>
+      </c>
+      <c r="F26" t="s">
+        <v>329</v>
+      </c>
+      <c r="G26" t="s">
+        <v>330</v>
+      </c>
+      <c r="H26" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" t="s">
+        <v>309</v>
+      </c>
+      <c r="F27" t="s">
+        <v>310</v>
+      </c>
+      <c r="G27" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>249</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D28" t="s">
+        <v>364</v>
+      </c>
+      <c r="E28" t="s">
+        <v>250</v>
+      </c>
+      <c r="F28" t="s">
+        <v>251</v>
+      </c>
+      <c r="G28" t="s">
+        <v>252</v>
+      </c>
+      <c r="H28" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>347</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D29" t="s">
+        <v>404</v>
+      </c>
+      <c r="E29" t="s">
+        <v>348</v>
+      </c>
+      <c r="F29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G29" t="s">
+        <v>350</v>
+      </c>
+      <c r="H29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>288</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D30" t="s">
+        <v>380</v>
+      </c>
+      <c r="E30" t="s">
+        <v>289</v>
+      </c>
+      <c r="F30" t="s">
+        <v>290</v>
+      </c>
+      <c r="G30" t="s">
+        <v>291</v>
+      </c>
+      <c r="H30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>293</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D31" t="s">
+        <v>382</v>
+      </c>
+      <c r="E31" t="s">
+        <v>294</v>
+      </c>
+      <c r="F31" t="s">
+        <v>295</v>
+      </c>
+      <c r="G31" t="s">
+        <v>296</v>
+      </c>
+      <c r="H31" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D32" t="s">
+        <v>372</v>
+      </c>
+      <c r="E32" t="s">
+        <v>270</v>
+      </c>
+      <c r="F32" t="s">
+        <v>271</v>
+      </c>
+      <c r="G32" t="s">
+        <v>272</v>
+      </c>
+      <c r="H32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H32" xr:uid="{195C5800-2193-C943-99C9-CAB091218E19}">
+    <sortState ref="A2:H32">
+      <sortCondition descending="1" ref="C1:C32"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE2C015-09BB-5C45-9873-75F289FC8FFC}">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A234" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
@@ -2653,704 +3770,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CEB70BC-EEE6-BF41-A547-15ABF05BD9E2}">
-  <dimension ref="A1:H26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2">
-        <v>0.64600536566280797</v>
-      </c>
-      <c r="D2">
-        <v>0.91888712345106005</v>
-      </c>
-      <c r="E2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G2" t="s">
-        <v>237</v>
-      </c>
-      <c r="H2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3">
-        <v>0.68736817392597604</v>
-      </c>
-      <c r="D3">
-        <v>0.85742686714534999</v>
-      </c>
-      <c r="E3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G3" t="s">
-        <v>242</v>
-      </c>
-      <c r="H3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4">
-        <v>0.74975215263685102</v>
-      </c>
-      <c r="D4">
-        <v>0.93225017431660895</v>
-      </c>
-      <c r="E4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F4" t="s">
-        <v>246</v>
-      </c>
-      <c r="G4" t="s">
-        <v>247</v>
-      </c>
-      <c r="H4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C5">
-        <v>0.56298238139188606</v>
-      </c>
-      <c r="D5">
-        <v>0.90685271154251801</v>
-      </c>
-      <c r="E5" t="s">
-        <v>250</v>
-      </c>
-      <c r="F5" t="s">
-        <v>251</v>
-      </c>
-      <c r="G5" t="s">
-        <v>252</v>
-      </c>
-      <c r="H5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6">
-        <v>0.66327628466280897</v>
-      </c>
-      <c r="D6">
-        <v>0.92400694170481001</v>
-      </c>
-      <c r="E6" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" t="s">
-        <v>256</v>
-      </c>
-      <c r="G6" t="s">
-        <v>257</v>
-      </c>
-      <c r="H6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C7">
-        <v>0.70477925600384095</v>
-      </c>
-      <c r="D7">
-        <v>0.90258689360558597</v>
-      </c>
-      <c r="E7" t="s">
-        <v>260</v>
-      </c>
-      <c r="F7" t="s">
-        <v>261</v>
-      </c>
-      <c r="G7" t="s">
-        <v>262</v>
-      </c>
-      <c r="H7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8">
-        <v>0.75251430821473797</v>
-      </c>
-      <c r="D8">
-        <v>0.92971130969772198</v>
-      </c>
-      <c r="E8" t="s">
-        <v>265</v>
-      </c>
-      <c r="F8" t="s">
-        <v>266</v>
-      </c>
-      <c r="G8" t="s">
-        <v>267</v>
-      </c>
-      <c r="H8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9">
-        <v>0.47624820403623902</v>
-      </c>
-      <c r="D9">
-        <v>0.72596409372302595</v>
-      </c>
-      <c r="E9" t="s">
-        <v>270</v>
-      </c>
-      <c r="F9" t="s">
-        <v>271</v>
-      </c>
-      <c r="G9" t="s">
-        <v>272</v>
-      </c>
-      <c r="H9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>273</v>
-      </c>
-      <c r="C10">
-        <v>0.63439978276519304</v>
-      </c>
-      <c r="D10">
-        <v>0.74868675713888</v>
-      </c>
-      <c r="E10" t="s">
-        <v>274</v>
-      </c>
-      <c r="F10" t="s">
-        <v>275</v>
-      </c>
-      <c r="G10" t="s">
-        <v>276</v>
-      </c>
-      <c r="H10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>278</v>
-      </c>
-      <c r="C11">
-        <v>0.69049463644454501</v>
-      </c>
-      <c r="D11">
-        <v>0.75939955018525895</v>
-      </c>
-      <c r="E11" t="s">
-        <v>279</v>
-      </c>
-      <c r="F11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G11" t="s">
-        <v>281</v>
-      </c>
-      <c r="H11" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>283</v>
-      </c>
-      <c r="C12">
-        <v>0.71432157780287497</v>
-      </c>
-      <c r="D12">
-        <v>0.76422108539761702</v>
-      </c>
-      <c r="E12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" t="s">
-        <v>285</v>
-      </c>
-      <c r="G12" t="s">
-        <v>286</v>
-      </c>
-      <c r="H12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C13">
-        <v>0.551704335502884</v>
-      </c>
-      <c r="D13">
-        <v>0.75990761154246</v>
-      </c>
-      <c r="E13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F13" t="s">
-        <v>290</v>
-      </c>
-      <c r="G13" t="s">
-        <v>291</v>
-      </c>
-      <c r="H13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>293</v>
-      </c>
-      <c r="C14">
-        <v>0.532538660509704</v>
-      </c>
-      <c r="D14">
-        <v>0.76181254388942998</v>
-      </c>
-      <c r="E14" t="s">
-        <v>294</v>
-      </c>
-      <c r="F14" t="s">
-        <v>295</v>
-      </c>
-      <c r="G14" t="s">
-        <v>296</v>
-      </c>
-      <c r="H14" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15">
-        <v>0.716063473796552</v>
-      </c>
-      <c r="D15">
-        <v>0.76919323398302897</v>
-      </c>
-      <c r="E15" t="s">
-        <v>299</v>
-      </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-      <c r="G15" t="s">
-        <v>301</v>
-      </c>
-      <c r="H15" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>303</v>
-      </c>
-      <c r="C16">
-        <v>0.72428717595434999</v>
-      </c>
-      <c r="D16">
-        <v>0.771189112636958</v>
-      </c>
-      <c r="E16" t="s">
-        <v>304</v>
-      </c>
-      <c r="F16" t="s">
-        <v>305</v>
-      </c>
-      <c r="G16" t="s">
-        <v>306</v>
-      </c>
-      <c r="H16" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>308</v>
-      </c>
-      <c r="C17">
-        <v>0.56497417242540604</v>
-      </c>
-      <c r="D17">
-        <v>0.63835548990644997</v>
-      </c>
-      <c r="E17" t="s">
-        <v>309</v>
-      </c>
-      <c r="F17" t="s">
-        <v>310</v>
-      </c>
-      <c r="G17" t="s">
-        <v>311</v>
-      </c>
-      <c r="H17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>312</v>
-      </c>
-      <c r="C18">
-        <v>0.70878803233047805</v>
-      </c>
-      <c r="D18">
-        <v>0.95180721895615406</v>
-      </c>
-      <c r="E18" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" t="s">
-        <v>314</v>
-      </c>
-      <c r="G18" t="s">
-        <v>315</v>
-      </c>
-      <c r="H18" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>317</v>
-      </c>
-      <c r="C19">
-        <v>0.72562431184922305</v>
-      </c>
-      <c r="D19">
-        <v>0.918361243135279</v>
-      </c>
-      <c r="E19" t="s">
-        <v>318</v>
-      </c>
-      <c r="F19" t="s">
-        <v>319</v>
-      </c>
-      <c r="G19" t="s">
-        <v>320</v>
-      </c>
-      <c r="H19" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>322</v>
-      </c>
-      <c r="C20">
-        <v>0.786587560569879</v>
-      </c>
-      <c r="D20">
-        <v>0.95058662552837903</v>
-      </c>
-      <c r="E20" t="s">
-        <v>323</v>
-      </c>
-      <c r="F20" t="s">
-        <v>324</v>
-      </c>
-      <c r="G20" t="s">
-        <v>325</v>
-      </c>
-      <c r="H20" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>327</v>
-      </c>
-      <c r="C21">
-        <v>0.63245422184567601</v>
-      </c>
-      <c r="D21">
-        <v>0.94704861583521405</v>
-      </c>
-      <c r="E21" t="s">
-        <v>328</v>
-      </c>
-      <c r="F21" t="s">
-        <v>329</v>
-      </c>
-      <c r="G21" t="s">
-        <v>330</v>
-      </c>
-      <c r="H21" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>332</v>
-      </c>
-      <c r="C22">
-        <v>0.71301449591863597</v>
-      </c>
-      <c r="D22">
-        <v>0.94908316414680405</v>
-      </c>
-      <c r="E22" t="s">
-        <v>333</v>
-      </c>
-      <c r="F22" t="s">
-        <v>334</v>
-      </c>
-      <c r="G22" t="s">
-        <v>335</v>
-      </c>
-      <c r="H22" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23">
-        <v>0.74540360526219496</v>
-      </c>
-      <c r="D23">
-        <v>0.93207686757521402</v>
-      </c>
-      <c r="E23" t="s">
-        <v>338</v>
-      </c>
-      <c r="F23" t="s">
-        <v>339</v>
-      </c>
-      <c r="G23" t="s">
-        <v>340</v>
-      </c>
-      <c r="H23" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>342</v>
-      </c>
-      <c r="C24">
-        <v>0.78500672715743502</v>
-      </c>
-      <c r="D24">
-        <v>0.95006076441791398</v>
-      </c>
-      <c r="E24" t="s">
-        <v>343</v>
-      </c>
-      <c r="F24" t="s">
-        <v>344</v>
-      </c>
-      <c r="G24" t="s">
-        <v>345</v>
-      </c>
-      <c r="H24" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>347</v>
-      </c>
-      <c r="C25">
-        <v>0.55495822047542398</v>
-      </c>
-      <c r="D25">
-        <v>0.762349495053811</v>
-      </c>
-      <c r="E25" t="s">
-        <v>348</v>
-      </c>
-      <c r="F25" t="s">
-        <v>349</v>
-      </c>
-      <c r="G25" t="s">
-        <v>350</v>
-      </c>
-      <c r="H25" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>352</v>
-      </c>
-      <c r="C26">
-        <v>0.70204695418984298</v>
-      </c>
-      <c r="D26">
-        <v>0.77369524614621299</v>
-      </c>
-      <c r="E26" t="s">
-        <v>353</v>
-      </c>
-      <c r="F26" t="s">
-        <v>354</v>
-      </c>
-      <c r="G26" t="s">
-        <v>355</v>
-      </c>
-      <c r="H26" t="s">
-        <v>356</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>